<commit_message>
calculate custom derived traits per cluster
</commit_message>
<xml_diff>
--- a/inst/extdata/traits_formulas.xlsx
+++ b/inst/extdata/traits_formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BB0F2C-263B-4D0E-90F6-049C7E75BA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099C3898-C07D-4D92-B069-AEF0FB51F6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23040" windowHeight="13898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>custom_trait = H3N4 + H3N4F1 + H4N4 + H4N4F1</t>
   </si>
   <si>
     <t>my_trait = (0.5 * H3N4 + H4N4) / (H3N4F1 + H4N4F1)</t>
+  </si>
+  <si>
+    <t>IgGI</t>
+  </si>
+  <si>
+    <t>IgGII</t>
   </si>
 </sst>
 </file>
@@ -348,21 +354,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
return custom traits in same format as normal traits. Includes columns with formulas
</commit_message>
<xml_diff>
--- a/inst/extdata/traits_formulas.xlsx
+++ b/inst/extdata/traits_formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099C3898-C07D-4D92-B069-AEF0FB51F6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187BA597-E2B8-467C-A7E3-95AD36E6D907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23040" windowHeight="13898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22714" yWindow="-231" windowWidth="23040" windowHeight="13897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>custom_trait = H3N4 + H3N4F1 + H4N4 + H4N4F1</t>
-  </si>
-  <si>
-    <t>my_trait = (0.5 * H3N4 + H4N4) / (H3N4F1 + H4N4F1)</t>
-  </si>
-  <si>
     <t>IgGI</t>
   </si>
   <si>
     <t>IgGII</t>
+  </si>
+  <si>
+    <t>first_trait = H3N4 + H3N4F1 + H4N4 + H4N4F1</t>
+  </si>
+  <si>
+    <t>second_trait = (0.5 * H3N4 + H4N4) / (H3N4F1 + H4N4F1)</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -367,18 +367,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>